<commit_message>
Created end-term result db view and added end-term results service implementation.
</commit_message>
<xml_diff>
--- a/SchoolPortal.Web/wwwroot/templates/Batch Upload Mid-Term Results Template.xlsx
+++ b/SchoolPortal.Web/wwwroot/templates/Batch Upload Mid-Term Results Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariofrancis\source\repos\SchoolPortal\SchoolPortal.Web\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60242FE7-06C2-4B16-93D7-409690BF8A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257EC4D1-6FF0-4302-B0D6-F0599CCB2928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{D4E0B7BB-266D-4FFE-864F-F1915E4699E5}"/>
+    <workbookView xWindow="2280" yWindow="750" windowWidth="19995" windowHeight="13125" xr2:uid="{D4E0B7BB-266D-4FFE-864F-F1915E4699E5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mid-Term Result Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -434,7 +434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>